<commit_message>
Latest version of the dashboard
</commit_message>
<xml_diff>
--- a/archive/Sorting/07-29Sorting Afternoon shift.xlsx
+++ b/archive/Sorting/07-29Sorting Afternoon shift.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,48 @@
   </si>
   <si>
     <t>Rates</t>
+  </si>
+  <si>
+    <t>Elia,Uruchima</t>
+  </si>
+  <si>
+    <t>Napoleon,Arnaud Hernandez</t>
+  </si>
+  <si>
+    <t>Luis,Vargas Jaquez</t>
+  </si>
+  <si>
+    <t>Edwin,Santos</t>
+  </si>
+  <si>
+    <t>Enmanuel,Vargas Rodriguez</t>
+  </si>
+  <si>
+    <t>Isaias,Basora Lugo</t>
+  </si>
+  <si>
+    <t>Madelyn,Rosario Moya</t>
+  </si>
+  <si>
+    <t>Anderson,Cespedes</t>
+  </si>
+  <si>
+    <t>Nancy,Ovillo</t>
+  </si>
+  <si>
+    <t>Edison,Rodriguez Gonzalez</t>
+  </si>
+  <si>
+    <t>Hansel,Reynoso</t>
+  </si>
+  <si>
+    <t>Jose,Correa</t>
+  </si>
+  <si>
+    <t>David ,Miranda Moncada</t>
+  </si>
+  <si>
+    <t>Aurelio,Mercedes Hernandez</t>
   </si>
   <si>
     <t>Total</t>
@@ -443,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,16 +531,16 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>187</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -510,10 +552,491 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>139.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>107</v>
+      </c>
+      <c r="K3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>94</v>
+      </c>
+      <c r="K4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>43</v>
+      </c>
+      <c r="I5">
+        <v>220</v>
+      </c>
+      <c r="J5">
+        <v>56</v>
+      </c>
+      <c r="K5">
+        <v>82.40000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>74</v>
+      </c>
+      <c r="D6">
+        <v>93</v>
+      </c>
+      <c r="E6">
+        <v>51</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>72.66666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>66</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>43</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>26</v>
+      </c>
+      <c r="K11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>507</v>
+      </c>
+      <c r="D16">
+        <v>310</v>
+      </c>
+      <c r="E16">
+        <v>240</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>43</v>
+      </c>
+      <c r="I16">
+        <v>220</v>
+      </c>
+      <c r="J16">
+        <v>375</v>
+      </c>
+      <c r="K16">
+        <v>171.1428571428571</v>
       </c>
     </row>
   </sheetData>
@@ -523,105 +1046,483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>74</v>
+      </c>
+      <c r="G2">
+        <v>66</v>
+      </c>
+      <c r="H2">
+        <v>55</v>
+      </c>
+      <c r="I2">
+        <v>43</v>
+      </c>
+      <c r="J2">
+        <v>41</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <v>507</v>
+      </c>
+      <c r="Q2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>93</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>19</v>
+      </c>
+      <c r="I3">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>310</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>51</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>240</v>
+      </c>
+      <c r="Q4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>43</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>43</v>
+      </c>
+      <c r="Q7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>220</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>220</v>
+      </c>
+      <c r="Q8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>107</v>
+      </c>
+      <c r="D9">
+        <v>94</v>
+      </c>
+      <c r="E9">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>26</v>
+      </c>
+      <c r="L9">
+        <v>25</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>375</v>
+      </c>
+      <c r="Q9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -640,19 +1541,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -660,19 +1561,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>246</v>
       </c>
       <c r="D2">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="F2">
-        <v>358</v>
+        <v>712</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -680,19 +1581,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C3">
-        <v>149</v>
+        <v>301</v>
       </c>
       <c r="D3">
-        <v>346</v>
+        <v>382</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="F3">
-        <v>495</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -700,19 +1601,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>392</v>
+        <v>643</v>
       </c>
       <c r="D4">
-        <v>611</v>
+        <v>661</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>683</v>
       </c>
       <c r="F4">
-        <v>1003</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -720,19 +1621,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>303</v>
+        <v>498</v>
       </c>
       <c r="D5">
-        <v>519</v>
+        <v>549</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>456</v>
       </c>
       <c r="F5">
-        <v>822</v>
+        <v>1503</v>
       </c>
     </row>
   </sheetData>
@@ -750,13 +1651,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -764,13 +1665,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2600</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1705</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>